<commit_message>
Updates to BOM, board design, and datasheets.
</commit_message>
<xml_diff>
--- a/docs/BOM.xlsx
+++ b/docs/BOM.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dan/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dan/Documents/eagle/dead10c5_2018/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB29F706-4B3C-474D-B62C-58BE46DCE621}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A743A76F-3C76-AD43-8A16-EA4ACF56E2D6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1620" windowWidth="25440" windowHeight="15000" xr2:uid="{1678DE2E-E161-724E-8C2F-7580DF32EE23}"/>
+    <workbookView xWindow="680" yWindow="2660" windowWidth="25440" windowHeight="15000" xr2:uid="{1678DE2E-E161-724E-8C2F-7580DF32EE23}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="50">
   <si>
     <t>Qty</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Mouser</t>
   </si>
   <si>
-    <t>COM-00536</t>
-  </si>
-  <si>
     <t>COM-09806</t>
   </si>
   <si>
@@ -84,12 +81,6 @@
     <t>10 Ohm resistor network</t>
   </si>
   <si>
-    <t>652-4607X-1LF-10</t>
-  </si>
-  <si>
-    <t>4607X-101-100LF</t>
-  </si>
-  <si>
     <t>Tactile Switch</t>
   </si>
   <si>
@@ -142,6 +133,48 @@
   </si>
   <si>
     <t>10-89-7061</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>COM-09661</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/9661</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/9806</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Microchip-Technology-Atmel/ATMEGA328P-PU?qs=sGAEpiMZZMtVoztFdqDXO6rEZqxeooRg</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/ABRACON/AWCR-1600MD?qs=%2fha2pyFadujFfudKd%2fAEbE32MTGIgZdnwSVrtFEweNr%2f82BKUq3Fzw%3d%3d</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Murata-Electronics/RDER71H104K0K1H03B?qs=%2fha2pyFadugsNiSzM4QtoPEqfGceYo24BOngKj3vXcmXztcZe0j46Uc%252bvWBqE1aS</t>
+  </si>
+  <si>
+    <t>652-4607X-1LF-330</t>
+  </si>
+  <si>
+    <t>4607X-101-331LF</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Bourns/4607X-101-331LF?qs=sGAEpiMZZMvrmc6UYKmaNWhNOGonlUnMh5dMy1XYfHQ%3d</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Panasonic/EVQ-PE604T?qs=%2fha2pyFadui45bz44%252bGA9GlcgqdKKtsWW4AUmDdzb54ngS0CtjvNBw%3d%3d</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Yageo/MFR-25FBF52-10K?qs=sGAEpiMZZMu61qfTUdNhG0IXHLFuiNnd4ZfMuxLN9bg%3d</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Molex/22-28-4060?qs=%2fha2pyFaduje7iG0C5h0B%2fdz9lYrXiF%2fSqnA9mKTPRg%2f8JanJs%2fc5A%3d%3d</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Molex/10-89-7061?qs=%2fha2pyFaduhUTuKyE5ihpKT%252bKedbNfhSu6VwpKmAGXgZ83GtknV09A%3d%3d</t>
   </si>
 </sst>
 </file>
@@ -149,7 +182,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -182,7 +215,7 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -503,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B560876-24AC-6F43-93B4-24DB3D996D6D}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -517,9 +550,10 @@
     <col min="5" max="5" width="13.1640625" customWidth="1"/>
     <col min="6" max="6" width="19.83203125" customWidth="1"/>
     <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="10" max="10" width="64.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -538,13 +572,16 @@
       </c>
       <c r="G1" s="3"/>
       <c r="H1" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -552,18 +589,19 @@
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>6</v>
       </c>
@@ -574,7 +612,7 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="E3" s="1">
         <f>7.95/25</f>
@@ -589,19 +627,22 @@
         <f>(25*7.55)</f>
         <v>188.75</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="1">
         <v>0.86</v>
@@ -615,20 +656,23 @@
         <f>100*A4*E4</f>
         <v>344</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G5" s="1">
         <v>1.84</v>
@@ -641,20 +685,23 @@
         <f>100*A5*G5</f>
         <v>184</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
         <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G6" s="1">
         <v>0.18</v>
@@ -667,20 +714,23 @@
         <f t="shared" ref="I6:I12" si="1">100*A6*G6</f>
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G7" s="1">
         <v>0.09</v>
@@ -693,44 +743,50 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="F8" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="G8" s="1">
-        <v>0.24099999999999999</v>
+        <v>0.255</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="0"/>
-        <v>0.24099999999999999</v>
+        <v>0.255</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="1"/>
-        <v>24.099999999999998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+        <v>25.5</v>
+      </c>
+      <c r="J8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G9" s="1">
         <v>0.33200000000000002</v>
@@ -743,19 +799,22 @@
         <f t="shared" si="1"/>
         <v>33.200000000000003</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" t="s">
         <v>29</v>
-      </c>
-      <c r="C10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" t="s">
-        <v>32</v>
       </c>
       <c r="G10" s="1">
         <v>0.02</v>
@@ -768,19 +827,22 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G11" s="1">
         <v>0.17299999999999999</v>
@@ -793,19 +855,22 @@
         <f t="shared" si="1"/>
         <v>17.299999999999997</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F12" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G12" s="1">
         <v>0.26600000000000001</v>
@@ -818,27 +883,31 @@
         <f t="shared" si="1"/>
         <v>26.6</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="H14" s="1">
         <f>SUM(H3:H13)</f>
-        <v>8.4899999999999984</v>
+        <v>8.5039999999999996</v>
       </c>
       <c r="I14" s="1">
         <f>SUM(I3:I13)</f>
-        <v>846.95</v>
+        <v>848.35</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="C1:C2"/>

</xml_diff>

<commit_message>
Added pic of Eagle rendering
</commit_message>
<xml_diff>
--- a/docs/BOM.xlsx
+++ b/docs/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dan/Documents/Projects/dead10c5_2018/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC728930-B872-CE47-8B1F-226B66F17A2C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96ACB2E2-0191-4A4A-8D64-1E747D550596}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="700" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{1678DE2E-E161-724E-8C2F-7580DF32EE23}"/>
+    <workbookView xWindow="160" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{1678DE2E-E161-724E-8C2F-7580DF32EE23}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="54">
   <si>
     <t>Qty</t>
   </si>
@@ -187,9 +187,6 @@
   </si>
   <si>
     <t>Price (qty 1)</t>
-  </si>
-  <si>
-    <t>Prototype</t>
   </si>
 </sst>
 </file>
@@ -246,10 +243,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -568,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B560876-24AC-6F43-93B4-24DB3D996D6D}">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G1:G1048576"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -585,39 +582,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4" t="s">
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4" t="s">
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
       <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
@@ -636,9 +633,9 @@
       <c r="I2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -670,7 +667,7 @@
         <f>(25*7.55)</f>
         <v>188.75</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="4" t="s">
         <v>38</v>
       </c>
     </row>
@@ -703,7 +700,7 @@
         <f>100*A4*F4</f>
         <v>344</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="L4" s="4" t="s">
         <v>39</v>
       </c>
     </row>
@@ -736,7 +733,7 @@
         <f>100*A5*I5</f>
         <v>184</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="L5" s="4" t="s">
         <v>40</v>
       </c>
     </row>
@@ -769,7 +766,7 @@
         <f t="shared" ref="K6:K13" si="1">100*A6*I6</f>
         <v>18</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="L6" s="4" t="s">
         <v>41</v>
       </c>
     </row>
@@ -802,7 +799,7 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="L7" s="5" t="s">
+      <c r="L7" s="4" t="s">
         <v>42</v>
       </c>
     </row>
@@ -834,7 +831,7 @@
         <f t="shared" si="1"/>
         <v>25.5</v>
       </c>
-      <c r="L8" s="5" t="s">
+      <c r="L8" s="4" t="s">
         <v>45</v>
       </c>
     </row>
@@ -866,7 +863,7 @@
         <f t="shared" si="1"/>
         <v>33.200000000000003</v>
       </c>
-      <c r="L9" s="5" t="s">
+      <c r="L9" s="4" t="s">
         <v>46</v>
       </c>
     </row>
@@ -898,7 +895,7 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="L10" s="5" t="s">
+      <c r="L10" s="4" t="s">
         <v>47</v>
       </c>
     </row>
@@ -930,7 +927,7 @@
         <f t="shared" si="1"/>
         <v>17.299999999999997</v>
       </c>
-      <c r="L11" s="5" t="s">
+      <c r="L11" s="4" t="s">
         <v>48</v>
       </c>
     </row>
@@ -962,7 +959,7 @@
         <f t="shared" si="1"/>
         <v>26.6</v>
       </c>
-      <c r="L12" s="5" t="s">
+      <c r="L12" s="4" t="s">
         <v>49</v>
       </c>
     </row>
@@ -994,7 +991,7 @@
         <f t="shared" si="1"/>
         <v>90.4</v>
       </c>
-      <c r="L13" s="5" t="s">
+      <c r="L13" s="4" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1011,7 +1008,7 @@
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I14" s="1">
         <f>J14</f>
@@ -1037,32 +1034,17 @@
         <v>1163.75</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>1</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="1">
-        <f>E3+(A4*E4)+SUM(H5:H13)</f>
-        <v>17.559999999999999</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B14:G14"/>
+  <mergeCells count="9">
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="B14:G14"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L13" r:id="rId1" xr:uid="{50942A3C-A0E3-A44A-BE84-1325492F9A7D}"/>

</xml_diff>

<commit_message>
Updated BOM with resistors for voltage divider to produce 3.3v
</commit_message>
<xml_diff>
--- a/docs/BOM.xlsx
+++ b/docs/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dan/Documents/Projects/dead10c5_2018/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96ACB2E2-0191-4A4A-8D64-1E747D550596}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F985A41-F106-3642-914D-702D5AE42271}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{1678DE2E-E161-724E-8C2F-7580DF32EE23}"/>
+    <workbookView xWindow="580" yWindow="1540" windowWidth="25440" windowHeight="15000" xr2:uid="{1678DE2E-E161-724E-8C2F-7580DF32EE23}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
   <si>
     <t>Qty</t>
   </si>
@@ -187,6 +187,18 @@
   </si>
   <si>
     <t>Price (qty 1)</t>
+  </si>
+  <si>
+    <t>3.6K Resistor</t>
+  </si>
+  <si>
+    <t>MBA02040C3601FC100</t>
+  </si>
+  <si>
+    <t>594-5063JD3.6K1%</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Vishay-Beyschlag/MBA02040C3601FC100?qs=Fjqjhfy7Xkq7TDUmKBbbFw%3d%3d</t>
   </si>
 </sst>
 </file>
@@ -565,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B560876-24AC-6F43-93B4-24DB3D996D6D}">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -759,11 +771,11 @@
         <v>0.18</v>
       </c>
       <c r="J6" s="1">
-        <f t="shared" ref="J6:J13" si="0">A6*I6</f>
+        <f t="shared" ref="J6:J14" si="0">A6*I6</f>
         <v>0.18</v>
       </c>
       <c r="K6" s="1">
-        <f t="shared" ref="K6:K13" si="1">100*A6*I6</f>
+        <f t="shared" ref="K6:K14" si="1">100*A6*I6</f>
         <v>18</v>
       </c>
       <c r="L6" s="4" t="s">
@@ -869,7 +881,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B10" t="s">
         <v>26</v>
@@ -889,11 +901,11 @@
       </c>
       <c r="J10" s="1">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="K10" s="1">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L10" s="4" t="s">
         <v>47</v>
@@ -904,31 +916,31 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="E11" s="1"/>
       <c r="G11" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="H11" s="1">
-        <v>0.23</v>
+        <v>0.11</v>
       </c>
       <c r="I11" s="1">
-        <v>0.17299999999999999</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="J11" s="1">
         <f t="shared" si="0"/>
-        <v>0.17299999999999999</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="K11" s="1">
         <f t="shared" si="1"/>
-        <v>17.299999999999997</v>
+        <v>8.1</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -936,31 +948,31 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E12" s="1"/>
       <c r="G12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H12" s="1">
-        <v>0.39</v>
+        <v>0.23</v>
       </c>
       <c r="I12" s="1">
-        <v>0.26600000000000001</v>
+        <v>0.17299999999999999</v>
       </c>
       <c r="J12" s="1">
         <f t="shared" si="0"/>
-        <v>0.26600000000000001</v>
+        <v>0.17299999999999999</v>
       </c>
       <c r="K12" s="1">
         <f t="shared" si="1"/>
-        <v>26.6</v>
+        <v>17.299999999999997</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -968,88 +980,120 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="E13" s="1"/>
       <c r="G13" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="H13" s="1">
-        <v>1.22</v>
+        <v>0.39</v>
       </c>
       <c r="I13" s="1">
-        <v>0.90400000000000003</v>
+        <v>0.26600000000000001</v>
       </c>
       <c r="J13" s="1">
         <f t="shared" si="0"/>
-        <v>0.90400000000000003</v>
+        <v>0.26600000000000001</v>
       </c>
       <c r="K13" s="1">
         <f t="shared" si="1"/>
-        <v>90.4</v>
+        <v>26.6</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="G14" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14" s="1">
+        <v>1.22</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0.90400000000000003</v>
+      </c>
+      <c r="J14" s="1">
+        <f t="shared" si="0"/>
+        <v>0.90400000000000003</v>
+      </c>
+      <c r="K14" s="1">
+        <f t="shared" si="1"/>
+        <v>90.4</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="1">
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="1">
         <v>10</v>
       </c>
-      <c r="I14" s="1">
-        <f>J14</f>
+      <c r="I15" s="1">
+        <f>J15</f>
         <v>2.25</v>
       </c>
-      <c r="J14" s="1">
-        <f>K14/100</f>
+      <c r="J15" s="1">
+        <f>K15/100</f>
         <v>2.25</v>
       </c>
-      <c r="K14" s="1">
+      <c r="K15" s="1">
         <v>225</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="E15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="J15" s="1">
-        <f>SUM(J3:J14)</f>
-        <v>11.657999999999999</v>
-      </c>
-      <c r="K15" s="1">
-        <f>SUM(K3:K14)</f>
-        <v>1163.75</v>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="E16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="J16" s="1">
+        <f>SUM(J3:J15)</f>
+        <v>11.758999999999999</v>
+      </c>
+      <c r="K16" s="1">
+        <f>SUM(K3:K15)</f>
+        <v>1173.8499999999999</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="B15:G15"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="B14:G14"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="L13" r:id="rId1" xr:uid="{50942A3C-A0E3-A44A-BE84-1325492F9A7D}"/>
-    <hyperlink ref="L12" r:id="rId2" xr:uid="{520AB970-801C-5D4F-93F7-2B4D5269F714}"/>
-    <hyperlink ref="L11" r:id="rId3" xr:uid="{36B1A202-2ACC-1540-8319-56FC0A67D35B}"/>
+    <hyperlink ref="L14" r:id="rId1" xr:uid="{50942A3C-A0E3-A44A-BE84-1325492F9A7D}"/>
+    <hyperlink ref="L13" r:id="rId2" xr:uid="{520AB970-801C-5D4F-93F7-2B4D5269F714}"/>
+    <hyperlink ref="L12" r:id="rId3" xr:uid="{36B1A202-2ACC-1540-8319-56FC0A67D35B}"/>
     <hyperlink ref="L10" r:id="rId4" xr:uid="{53BE59D8-4830-9143-BE73-BC73F5389FA0}"/>
     <hyperlink ref="L9" r:id="rId5" xr:uid="{AE102F7D-522B-EA4F-9D37-A755ABDC2340}"/>
     <hyperlink ref="L8" r:id="rId6" xr:uid="{8052FECB-29BF-9140-943B-F26F54E8A435}"/>

</xml_diff>